<commit_message>
plot health outcome v2
</commit_message>
<xml_diff>
--- a/data/extraction_grid_health_outcome.xlsx
+++ b/data/extraction_grid_health_outcome.xlsx
@@ -882,9 +882,6 @@
     <t>Climate policies can help resolve energy security and air pollution chAllenges</t>
   </si>
   <si>
-    <t>Global</t>
-  </si>
-  <si>
     <t>Energy, transport, industry, agriculture</t>
   </si>
   <si>
@@ -910,6 +907,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>All-encompassing</t>
   </si>
 </sst>
 </file>
@@ -2338,9 +2338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA8" sqref="AA8"/>
+      <selection pane="topRight" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2438,7 +2438,7 @@
         <v>281</v>
       </c>
       <c r="AA1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="144.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2518,7 +2518,7 @@
         <v>279</v>
       </c>
       <c r="AA2" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="31" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -2591,7 +2591,7 @@
         <v>279</v>
       </c>
       <c r="AA3" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:27" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2617,10 +2617,10 @@
         <v>125</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>207</v>
@@ -2664,7 +2664,7 @@
         <v>278</v>
       </c>
       <c r="AA4" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="31" customFormat="1" ht="250.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2690,10 +2690,10 @@
         <v>125</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>207</v>
@@ -2737,7 +2737,7 @@
         <v>278</v>
       </c>
       <c r="AA5" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:27" s="31" customFormat="1" ht="218.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2763,10 +2763,10 @@
         <v>125</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>207</v>
@@ -2810,7 +2810,7 @@
         <v>278</v>
       </c>
       <c r="AA6" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:27" s="31" customFormat="1" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2875,7 +2875,7 @@
         <v>278</v>
       </c>
       <c r="AA7" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:27" s="28" customFormat="1" ht="220.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2930,7 +2930,7 @@
         <v>278</v>
       </c>
       <c r="AA8" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:27" s="79" customFormat="1" ht="289.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2956,7 +2956,7 @@
         <v>188</v>
       </c>
       <c r="H9" s="73" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I9" s="73" t="s">
         <v>263</v>
@@ -2997,7 +2997,7 @@
         <v>278</v>
       </c>
       <c r="AA9" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:27" s="79" customFormat="1" ht="289.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3023,7 +3023,7 @@
         <v>188</v>
       </c>
       <c r="H10" s="73" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I10" s="73" t="s">
         <v>263</v>
@@ -3064,7 +3064,7 @@
         <v>278</v>
       </c>
       <c r="AA10" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:27" s="79" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3090,7 +3090,7 @@
         <v>188</v>
       </c>
       <c r="H11" s="73" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I11" s="73" t="s">
         <v>263</v>
@@ -3131,7 +3131,7 @@
         <v>278</v>
       </c>
       <c r="AA11" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:27" s="79" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3157,7 +3157,7 @@
         <v>188</v>
       </c>
       <c r="H12" s="73" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I12" s="73" t="s">
         <v>263</v>
@@ -3198,7 +3198,7 @@
         <v>278</v>
       </c>
       <c r="AA12" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:27" s="79" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -3222,10 +3222,10 @@
         <v>188</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I13" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>208</v>
@@ -3251,7 +3251,7 @@
         <v>280</v>
       </c>
       <c r="AA13" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3315,7 +3315,7 @@
         <v>278</v>
       </c>
       <c r="AA14" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3379,7 +3379,7 @@
         <v>278</v>
       </c>
       <c r="AA15" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3443,7 +3443,7 @@
         <v>278</v>
       </c>
       <c r="AA16" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3507,7 +3507,7 @@
         <v>278</v>
       </c>
       <c r="AA17" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3571,7 +3571,7 @@
         <v>278</v>
       </c>
       <c r="AA18" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3635,7 +3635,7 @@
         <v>278</v>
       </c>
       <c r="AA19" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:27" s="38" customFormat="1" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3701,7 +3701,7 @@
         <v>278</v>
       </c>
       <c r="AA20" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:27" s="38" customFormat="1" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3766,7 +3766,7 @@
         <v>278</v>
       </c>
       <c r="AA21" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:27" s="38" customFormat="1" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3819,7 +3819,7 @@
         <v>278</v>
       </c>
       <c r="AA22" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:27" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3845,7 +3845,7 @@
         <v>125</v>
       </c>
       <c r="H23" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I23" s="35" t="s">
         <v>263</v>
@@ -3883,7 +3883,7 @@
         <v>278</v>
       </c>
       <c r="AA23" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="1:27" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3909,7 +3909,7 @@
         <v>125</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I24" s="35" t="s">
         <v>263</v>
@@ -3947,7 +3947,7 @@
         <v>278</v>
       </c>
       <c r="AA24" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:27" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -4002,7 +4002,7 @@
         <v>278</v>
       </c>
       <c r="AA25" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:27" s="31" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -4026,7 +4026,7 @@
         <v>188</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>263</v>
@@ -4055,7 +4055,7 @@
         <v>278</v>
       </c>
       <c r="AA26" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:27" s="31" customFormat="1" ht="216" customHeight="1" x14ac:dyDescent="0.3">
@@ -4081,10 +4081,10 @@
         <v>188</v>
       </c>
       <c r="H27" s="73" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I27" s="73" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J27" s="77" t="s">
         <v>207</v>
@@ -4120,7 +4120,7 @@
         <v>278</v>
       </c>
       <c r="AA27" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:27" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4173,7 +4173,7 @@
         <v>278</v>
       </c>
       <c r="AA28" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:27" s="79" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4248,7 +4248,7 @@
         <v>279</v>
       </c>
       <c r="AA29" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:27" s="31" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4323,7 +4323,7 @@
         <v>279</v>
       </c>
       <c r="AA30" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:27" s="79" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4398,7 +4398,7 @@
         <v>279</v>
       </c>
       <c r="AA31" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:27" s="79" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4473,7 +4473,7 @@
         <v>279</v>
       </c>
       <c r="AA32" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="33" spans="1:27" s="79" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4548,7 +4548,7 @@
         <v>279</v>
       </c>
       <c r="AA33" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:27" s="79" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4623,7 +4623,7 @@
         <v>279</v>
       </c>
       <c r="AA34" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:27" s="79" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4698,7 +4698,7 @@
         <v>279</v>
       </c>
       <c r="AA35" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="1:27" s="79" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4773,7 +4773,7 @@
         <v>279</v>
       </c>
       <c r="AA36" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="1:27" s="79" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4837,7 +4837,7 @@
         <v>278</v>
       </c>
       <c r="AA37" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:27" s="79" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4909,7 +4909,7 @@
         <v>279</v>
       </c>
       <c r="AA38" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:27" s="31" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -4974,7 +4974,7 @@
         <v>278</v>
       </c>
       <c r="AA39" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:27" s="31" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -5039,7 +5039,7 @@
         <v>278</v>
       </c>
       <c r="AA40" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="41" spans="1:27" s="28" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -5104,7 +5104,7 @@
         <v>278</v>
       </c>
       <c r="AA41" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:27" s="28" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -5169,7 +5169,7 @@
         <v>278</v>
       </c>
       <c r="AA42" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="43" spans="1:27" s="28" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -5234,7 +5234,7 @@
         <v>278</v>
       </c>
       <c r="AA43" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" spans="1:27" s="28" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -5299,7 +5299,7 @@
         <v>278</v>
       </c>
       <c r="AA44" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="45" spans="1:27" s="28" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
@@ -5365,7 +5365,7 @@
         <v>278</v>
       </c>
       <c r="AA45" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" spans="1:27" s="28" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
@@ -5431,7 +5431,7 @@
         <v>279</v>
       </c>
       <c r="AA46" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" spans="1:27" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5496,7 +5496,7 @@
         <v>278</v>
       </c>
       <c r="AA47" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:27" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5561,7 +5561,7 @@
         <v>278</v>
       </c>
       <c r="AA48" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5626,7 +5626,7 @@
         <v>278</v>
       </c>
       <c r="AA49" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5691,7 +5691,7 @@
         <v>278</v>
       </c>
       <c r="AA50" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="1:27" s="28" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -5755,7 +5755,7 @@
         <v>278</v>
       </c>
       <c r="AA51" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:27" s="28" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5781,10 +5781,10 @@
         <v>188</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>207</v>
@@ -5819,7 +5819,7 @@
         <v>278</v>
       </c>
       <c r="AA52" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:27" s="31" customFormat="1" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5845,10 +5845,10 @@
         <v>188</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J53" s="8" t="s">
         <v>207</v>
@@ -5883,7 +5883,7 @@
         <v>278</v>
       </c>
       <c r="AA53" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="54" spans="1:27" s="31" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -5909,10 +5909,10 @@
         <v>188</v>
       </c>
       <c r="H54" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J54" s="65" t="s">
         <v>207</v>
@@ -5947,7 +5947,7 @@
         <v>278</v>
       </c>
       <c r="AA54" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="55" spans="1:27" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5973,10 +5973,10 @@
         <v>155</v>
       </c>
       <c r="H55" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J55" s="65" t="s">
         <v>207</v>
@@ -6011,7 +6011,7 @@
         <v>278</v>
       </c>
       <c r="AA55" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="56" spans="1:27" s="28" customFormat="1" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6037,10 +6037,10 @@
         <v>155</v>
       </c>
       <c r="H56" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I56" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J56" s="65" t="s">
         <v>207</v>
@@ -6075,7 +6075,7 @@
         <v>278</v>
       </c>
       <c r="AA56" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" spans="1:27" s="28" customFormat="1" ht="225.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6139,7 +6139,7 @@
         <v>278</v>
       </c>
       <c r="AA57" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="58" spans="1:27" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -6203,7 +6203,7 @@
         <v>278</v>
       </c>
       <c r="AA58" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="1:27" s="28" customFormat="1" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -6267,7 +6267,7 @@
         <v>278</v>
       </c>
       <c r="AA59" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="1:27" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -6331,7 +6331,7 @@
         <v>278</v>
       </c>
       <c r="AA60" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="61" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6357,7 +6357,7 @@
         <v>188</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I61" s="15" t="s">
         <v>263</v>
@@ -6395,7 +6395,7 @@
         <v>278</v>
       </c>
       <c r="AA61" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6421,7 +6421,7 @@
         <v>135</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I62" s="15" t="s">
         <v>263</v>
@@ -6460,7 +6460,7 @@
         <v>278</v>
       </c>
       <c r="AA62" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:27" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6486,7 +6486,7 @@
         <v>188</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I63" s="15" t="s">
         <v>263</v>
@@ -6524,7 +6524,7 @@
         <v>278</v>
       </c>
       <c r="AA63" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="1:27" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6550,7 +6550,7 @@
         <v>135</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>263</v>
@@ -6589,7 +6589,7 @@
         <v>278</v>
       </c>
       <c r="AA64" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" spans="1:27" s="19" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
@@ -6642,7 +6642,7 @@
         <v>278</v>
       </c>
       <c r="AA65" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="66" spans="1:27" s="19" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -6668,7 +6668,7 @@
         <v>188</v>
       </c>
       <c r="H66" s="35" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I66" s="35" t="s">
         <v>263</v>
@@ -6717,7 +6717,7 @@
         <v>278</v>
       </c>
       <c r="AA66" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="67" spans="1:27" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -6743,10 +6743,10 @@
         <v>188</v>
       </c>
       <c r="H67" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I67" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J67" s="65" t="s">
         <v>207</v>
@@ -6782,7 +6782,7 @@
         <v>278</v>
       </c>
       <c r="AA67" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="68" spans="1:27" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -6808,10 +6808,10 @@
         <v>188</v>
       </c>
       <c r="H68" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J68" s="65" t="s">
         <v>207</v>
@@ -6858,7 +6858,7 @@
         <v>278</v>
       </c>
       <c r="AA68" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:27" s="28" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -6922,7 +6922,7 @@
         <v>279</v>
       </c>
       <c r="AA69" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="70" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6948,10 +6948,10 @@
         <v>188</v>
       </c>
       <c r="H70" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I70" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J70" s="65" t="s">
         <v>207</v>
@@ -6996,7 +6996,7 @@
         <v>278</v>
       </c>
       <c r="AA70" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7022,10 +7022,10 @@
         <v>188</v>
       </c>
       <c r="H71" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I71" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J71" s="65" t="s">
         <v>207</v>
@@ -7061,7 +7061,7 @@
         <v>278</v>
       </c>
       <c r="AA71" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="72" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7087,10 +7087,10 @@
         <v>188</v>
       </c>
       <c r="H72" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I72" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J72" s="65" t="s">
         <v>207</v>
@@ -7135,7 +7135,7 @@
         <v>278</v>
       </c>
       <c r="AA72" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="73" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7161,10 +7161,10 @@
         <v>125</v>
       </c>
       <c r="H73" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I73" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J73" s="65" t="s">
         <v>207</v>
@@ -7200,7 +7200,7 @@
         <v>278</v>
       </c>
       <c r="AA73" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="74" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7226,10 +7226,10 @@
         <v>125</v>
       </c>
       <c r="H74" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I74" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J74" s="65" t="s">
         <v>207</v>
@@ -7265,7 +7265,7 @@
         <v>278</v>
       </c>
       <c r="AA74" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="75" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7291,10 +7291,10 @@
         <v>125</v>
       </c>
       <c r="H75" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I75" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J75" s="65" t="s">
         <v>207</v>
@@ -7330,7 +7330,7 @@
         <v>278</v>
       </c>
       <c r="AA75" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="76" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7356,10 +7356,10 @@
         <v>125</v>
       </c>
       <c r="H76" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I76" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J76" s="65" t="s">
         <v>207</v>
@@ -7395,7 +7395,7 @@
         <v>278</v>
       </c>
       <c r="AA76" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="77" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7421,10 +7421,10 @@
         <v>125</v>
       </c>
       <c r="H77" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I77" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J77" s="65" t="s">
         <v>207</v>
@@ -7460,7 +7460,7 @@
         <v>278</v>
       </c>
       <c r="AA77" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="78" spans="1:27" s="66" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7486,10 +7486,10 @@
         <v>125</v>
       </c>
       <c r="H78" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I78" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J78" s="65" t="s">
         <v>207</v>
@@ -7525,7 +7525,7 @@
         <v>278</v>
       </c>
       <c r="AA78" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="79" spans="1:27" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7590,7 +7590,7 @@
         <v>279</v>
       </c>
       <c r="AA79" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="80" spans="1:27" s="28" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7616,10 +7616,10 @@
         <v>188</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J80" s="8" t="s">
         <v>207</v>
@@ -7663,7 +7663,7 @@
         <v>278</v>
       </c>
       <c r="AA80" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" spans="1:27" s="31" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.3">
@@ -7689,10 +7689,10 @@
         <v>188</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J81" s="8" t="s">
         <v>207</v>
@@ -7736,7 +7736,7 @@
         <v>278</v>
       </c>
       <c r="AA81" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="82" spans="1:27" s="31" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.3">
@@ -7762,10 +7762,10 @@
         <v>188</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J82" s="8" t="s">
         <v>207</v>
@@ -7809,7 +7809,7 @@
         <v>278</v>
       </c>
       <c r="AA82" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="83" spans="1:27" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7867,7 +7867,7 @@
         <v>278</v>
       </c>
       <c r="AA83" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:27" s="31" customFormat="1" ht="222.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -7940,7 +7940,7 @@
         <v>279</v>
       </c>
       <c r="AA84" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:27" s="28" customFormat="1" ht="223.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -7966,10 +7966,10 @@
         <v>125</v>
       </c>
       <c r="H85" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I85" s="35" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="J85" s="65" t="s">
         <v>207</v>
@@ -8013,7 +8013,7 @@
         <v>279</v>
       </c>
       <c r="AA85" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="86" spans="1:27" s="70" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8079,7 +8079,7 @@
         <v>278</v>
       </c>
       <c r="AA86" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="87" spans="1:27" s="70" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8105,7 +8105,7 @@
         <v>135</v>
       </c>
       <c r="H87" s="35" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I87" s="35" t="s">
         <v>263</v>
@@ -8152,7 +8152,7 @@
         <v>278</v>
       </c>
       <c r="AA87" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="88" spans="1:27" s="28" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -8217,7 +8217,7 @@
         <v>278</v>
       </c>
       <c r="AA88" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="89" spans="1:27" s="28" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -8282,7 +8282,7 @@
         <v>278</v>
       </c>
       <c r="AA89" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="1:27" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8337,7 +8337,7 @@
         <v>278</v>
       </c>
       <c r="AA90" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="91" spans="1:27" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8403,7 +8403,7 @@
         <v>278</v>
       </c>
       <c r="AA91" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="92" spans="1:27" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8469,7 +8469,7 @@
         <v>278</v>
       </c>
       <c r="AA92" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="93" spans="1:27" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8535,7 +8535,7 @@
         <v>278</v>
       </c>
       <c r="AA93" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="94" spans="1:27" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8600,7 +8600,7 @@
         <v>279</v>
       </c>
       <c r="AA94" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:27" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8665,7 +8665,7 @@
         <v>279</v>
       </c>
       <c r="AA95" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="96" spans="1:27" s="28" customFormat="1" ht="176.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -8691,7 +8691,7 @@
         <v>188</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I96" s="5" t="s">
         <v>263</v>
@@ -8730,7 +8730,7 @@
         <v>279</v>
       </c>
       <c r="AA96" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="97" spans="1:27" s="31" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.3">
@@ -8756,7 +8756,7 @@
         <v>188</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I97" s="5" t="s">
         <v>263</v>
@@ -8795,7 +8795,7 @@
         <v>279</v>
       </c>
       <c r="AA97" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="98" spans="1:27" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8877,7 +8877,7 @@
         <v>278</v>
       </c>
       <c r="AA98" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="99" spans="1:27" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8943,7 +8943,7 @@
         <v>278</v>
       </c>
       <c r="AA99" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="100" spans="1:27" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -9009,7 +9009,7 @@
         <v>278</v>
       </c>
       <c r="AA100" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="101" spans="1:27" s="28" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -9075,7 +9075,7 @@
         <v>278</v>
       </c>
       <c r="AA101" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="102" spans="1:27" s="28" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -9141,7 +9141,7 @@
         <v>278</v>
       </c>
       <c r="AA102" s="97" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>